<commit_message>
complete constraints with functions of phase#1
</commit_message>
<xml_diff>
--- a/rules/DMAVTYM_Alles_V1_0.xlsx
+++ b/rules/DMAVTYM_Alles_V1_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SOURCE\DMAV-Validierungsmodell\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6134B727-1611-4203-B567-E048E6679034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FE643E-151C-4B57-8703-16B1597729BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="240" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,20 @@
     <definedName name="Statistics">#REF!</definedName>
     <definedName name="Version">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2692,13 +2705,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:S181" totalsRowShown="0" dataDxfId="19">
-  <autoFilter ref="A1:S181" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="12">
-      <customFilters>
-        <customFilter val="*Gemeindegrenze*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S181" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S181">
     <sortCondition ref="S1:S181"/>
   </sortState>
@@ -3062,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A85" sqref="A80:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,7 +3155,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3184,7 +3191,7 @@
       </c>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3231,7 +3238,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3278,7 +3285,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3325,7 +3332,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3372,7 +3379,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3419,7 +3426,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3466,7 +3473,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3513,7 +3520,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3560,7 +3567,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3607,7 +3614,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3654,7 +3661,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3697,7 +3704,7 @@
       <c r="R13"/>
       <c r="S13" s="13"/>
     </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3744,7 +3751,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3791,7 +3798,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3838,7 +3845,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3879,7 +3886,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3920,7 +3927,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3961,7 +3968,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4002,7 +4009,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4043,7 +4050,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4084,7 +4091,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4125,7 +4132,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4166,7 +4173,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4207,7 +4214,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -4251,7 +4258,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4289,7 +4296,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -4328,7 +4335,7 @@
       </c>
       <c r="S28" s="12"/>
     </row>
-    <row r="29" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -4367,7 +4374,7 @@
       </c>
       <c r="S29" s="12"/>
     </row>
-    <row r="30" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -4403,7 +4410,7 @@
       </c>
       <c r="S30" s="12"/>
     </row>
-    <row r="31" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -4439,7 +4446,7 @@
       </c>
       <c r="S31" s="12"/>
     </row>
-    <row r="32" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -4475,7 +4482,7 @@
       </c>
       <c r="S32" s="12"/>
     </row>
-    <row r="33" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -4511,7 +4518,7 @@
       </c>
       <c r="S33" s="12"/>
     </row>
-    <row r="34" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -4547,7 +4554,7 @@
       </c>
       <c r="S34" s="12"/>
     </row>
-    <row r="35" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4583,7 +4590,7 @@
       </c>
       <c r="S35" s="12"/>
     </row>
-    <row r="36" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4619,7 +4626,7 @@
       </c>
       <c r="S36" s="12"/>
     </row>
-    <row r="37" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -4655,7 +4662,7 @@
       </c>
       <c r="S37" s="12"/>
     </row>
-    <row r="38" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -4691,7 +4698,7 @@
       </c>
       <c r="S38" s="12"/>
     </row>
-    <row r="39" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4730,7 +4737,7 @@
       </c>
       <c r="S39" s="12"/>
     </row>
-    <row r="40" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -4766,7 +4773,7 @@
       </c>
       <c r="S40" s="12"/>
     </row>
-    <row r="41" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4802,7 +4809,7 @@
       </c>
       <c r="S41" s="12"/>
     </row>
-    <row r="42" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -4841,7 +4848,7 @@
       </c>
       <c r="S42" s="12"/>
     </row>
-    <row r="43" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4880,7 +4887,7 @@
       </c>
       <c r="S43" s="12"/>
     </row>
-    <row r="44" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4919,7 +4926,7 @@
       </c>
       <c r="S44" s="12"/>
     </row>
-    <row r="45" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4958,7 +4965,7 @@
       </c>
       <c r="S45" s="12"/>
     </row>
-    <row r="46" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4997,7 +5004,7 @@
       </c>
       <c r="S46" s="12"/>
     </row>
-    <row r="47" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -5036,7 +5043,7 @@
       </c>
       <c r="S47" s="12"/>
     </row>
-    <row r="48" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5072,7 +5079,7 @@
       </c>
       <c r="S48" s="12"/>
     </row>
-    <row r="49" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -5108,7 +5115,7 @@
       </c>
       <c r="S49" s="12"/>
     </row>
-    <row r="50" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -5144,7 +5151,7 @@
       </c>
       <c r="S50" s="12"/>
     </row>
-    <row r="51" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -5180,7 +5187,7 @@
       </c>
       <c r="S51" s="12"/>
     </row>
-    <row r="52" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -5219,7 +5226,7 @@
       </c>
       <c r="S52" s="12"/>
     </row>
-    <row r="53" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -5258,7 +5265,7 @@
       </c>
       <c r="S53" s="12"/>
     </row>
-    <row r="54" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -5294,7 +5301,7 @@
       </c>
       <c r="S54" s="12"/>
     </row>
-    <row r="55" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -5330,7 +5337,7 @@
       </c>
       <c r="S55" s="12"/>
     </row>
-    <row r="56" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -5366,7 +5373,7 @@
       </c>
       <c r="S56" s="12"/>
     </row>
-    <row r="57" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -5402,7 +5409,7 @@
       </c>
       <c r="S57" s="12"/>
     </row>
-    <row r="58" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -5441,7 +5448,7 @@
       </c>
       <c r="S58" s="12"/>
     </row>
-    <row r="59" spans="1:19" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>12</v>
       </c>
@@ -5477,7 +5484,7 @@
       </c>
       <c r="S59" s="13"/>
     </row>
-    <row r="60" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -5513,7 +5520,7 @@
       </c>
       <c r="S60" s="12"/>
     </row>
-    <row r="61" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -5549,7 +5556,7 @@
       </c>
       <c r="S61" s="12"/>
     </row>
-    <row r="62" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -5585,7 +5592,7 @@
       </c>
       <c r="S62" s="12"/>
     </row>
-    <row r="63" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -5624,7 +5631,7 @@
       </c>
       <c r="S63" s="12"/>
     </row>
-    <row r="64" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -5663,7 +5670,7 @@
       </c>
       <c r="S64" s="12"/>
     </row>
-    <row r="65" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -5702,7 +5709,7 @@
       </c>
       <c r="S65" s="12"/>
     </row>
-    <row r="66" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -5740,7 +5747,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -5779,7 +5786,7 @@
       </c>
       <c r="S67" s="12"/>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -5817,7 +5824,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -5853,7 +5860,7 @@
       </c>
       <c r="S69" s="12"/>
     </row>
-    <row r="70" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -5891,7 +5898,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -5932,7 +5939,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -5971,7 +5978,7 @@
       </c>
       <c r="S72" s="12"/>
     </row>
-    <row r="73" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -6007,7 +6014,7 @@
       </c>
       <c r="S73" s="12"/>
     </row>
-    <row r="74" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -6046,7 +6053,7 @@
       </c>
       <c r="S74" s="12"/>
     </row>
-    <row r="75" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -6084,7 +6091,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -6122,7 +6129,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -6161,7 +6168,7 @@
       </c>
       <c r="S77" s="12"/>
     </row>
-    <row r="78" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -6199,7 +6206,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="79" spans="1:19" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>12</v>
       </c>
@@ -6235,7 +6242,7 @@
       </c>
       <c r="S79" s="13"/>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -6311,7 +6318,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -6393,7 +6400,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -6431,7 +6438,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -6472,7 +6479,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -6516,7 +6523,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -6554,7 +6561,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -6593,7 +6600,7 @@
       </c>
       <c r="S88" s="12"/>
     </row>
-    <row r="89" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -6629,7 +6636,7 @@
       </c>
       <c r="S89" s="12"/>
     </row>
-    <row r="90" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -6670,7 +6677,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -6706,7 +6713,7 @@
       </c>
       <c r="S91" s="12"/>
     </row>
-    <row r="92" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -6750,7 +6757,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -6786,7 +6793,7 @@
       </c>
       <c r="S93" s="12"/>
     </row>
-    <row r="94" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>12</v>
       </c>
@@ -6822,7 +6829,7 @@
       </c>
       <c r="S94" s="13"/>
     </row>
-    <row r="95" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
@@ -6858,7 +6865,7 @@
       </c>
       <c r="S95" s="13"/>
     </row>
-    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -6896,7 +6903,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -6934,7 +6941,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -6972,7 +6979,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="99" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -7010,7 +7017,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -7048,7 +7055,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -7086,7 +7093,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -7124,7 +7131,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="103" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>12</v>
       </c>
@@ -7160,7 +7167,7 @@
       </c>
       <c r="S103" s="13"/>
     </row>
-    <row r="104" spans="1:19" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>12</v>
       </c>
@@ -7196,7 +7203,7 @@
       </c>
       <c r="S104" s="13"/>
     </row>
-    <row r="105" spans="1:19" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>12</v>
       </c>
@@ -7232,7 +7239,7 @@
       </c>
       <c r="S105" s="13"/>
     </row>
-    <row r="106" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -7270,7 +7277,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>12</v>
       </c>
@@ -7308,7 +7315,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -7346,7 +7353,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -7384,7 +7391,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="110" spans="1:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F110" s="3" t="s">
         <v>456</v>
       </c>
@@ -7397,7 +7404,7 @@
       <c r="O110" s="8"/>
       <c r="S110" s="12"/>
     </row>
-    <row r="111" spans="1:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F111" s="3" t="s">
         <v>457</v>
       </c>
@@ -7410,7 +7417,7 @@
       <c r="O111" s="6"/>
       <c r="S111" s="12"/>
     </row>
-    <row r="112" spans="1:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F112" s="3" t="s">
         <v>458</v>
       </c>
@@ -7423,7 +7430,7 @@
       <c r="O112" s="6"/>
       <c r="S112" s="12"/>
     </row>
-    <row r="113" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F113" s="3" t="s">
         <v>459</v>
       </c>
@@ -7436,7 +7443,7 @@
       <c r="O113" s="6"/>
       <c r="S113" s="12"/>
     </row>
-    <row r="114" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F114" s="3" t="s">
         <v>460</v>
       </c>
@@ -7449,7 +7456,7 @@
       <c r="O114" s="6"/>
       <c r="S114" s="12"/>
     </row>
-    <row r="115" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F115" s="3" t="s">
         <v>461</v>
       </c>
@@ -7462,7 +7469,7 @@
       <c r="O115" s="6"/>
       <c r="S115" s="12"/>
     </row>
-    <row r="116" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F116" s="3" t="s">
         <v>462</v>
       </c>
@@ -7475,7 +7482,7 @@
       <c r="O116" s="6"/>
       <c r="S116" s="12"/>
     </row>
-    <row r="117" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F117" s="3" t="s">
         <v>463</v>
       </c>
@@ -7488,7 +7495,7 @@
       <c r="O117" s="6"/>
       <c r="S117" s="12"/>
     </row>
-    <row r="118" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F118" s="3" t="s">
         <v>464</v>
       </c>
@@ -7501,7 +7508,7 @@
       <c r="O118" s="6"/>
       <c r="S118" s="12"/>
     </row>
-    <row r="119" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F119" s="3" t="s">
         <v>465</v>
       </c>
@@ -7514,7 +7521,7 @@
       <c r="O119" s="6"/>
       <c r="S119" s="12"/>
     </row>
-    <row r="120" spans="6:19" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="6:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F120" s="3" t="s">
         <v>466</v>
       </c>
@@ -7592,7 +7599,7 @@
       <c r="O125" s="6"/>
       <c r="S125" s="12"/>
     </row>
-    <row r="126" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F126" s="3" t="s">
         <v>472</v>
       </c>
@@ -7605,7 +7612,7 @@
       <c r="O126" s="6"/>
       <c r="S126" s="12"/>
     </row>
-    <row r="127" spans="6:19" s="3" customFormat="1" ht="72.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="6:19" s="3" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F127" s="3" t="s">
         <v>473</v>
       </c>
@@ -7618,7 +7625,7 @@
       <c r="O127" s="6"/>
       <c r="S127" s="12"/>
     </row>
-    <row r="128" spans="6:19" s="3" customFormat="1" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="6:19" s="3" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F128" s="3" t="s">
         <v>474</v>
       </c>
@@ -7631,7 +7638,7 @@
       <c r="O128" s="6"/>
       <c r="S128" s="12"/>
     </row>
-    <row r="129" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F129" s="3" t="s">
         <v>475</v>
       </c>
@@ -7644,7 +7651,7 @@
       <c r="O129" s="6"/>
       <c r="S129" s="12"/>
     </row>
-    <row r="130" spans="6:19" s="3" customFormat="1" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="6:19" s="3" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F130" s="3" t="s">
         <v>476</v>
       </c>
@@ -7657,7 +7664,7 @@
       <c r="O130" s="6"/>
       <c r="S130" s="12"/>
     </row>
-    <row r="131" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F131" s="3" t="s">
         <v>477</v>
       </c>
@@ -7670,7 +7677,7 @@
       <c r="O131" s="10"/>
       <c r="S131" s="12"/>
     </row>
-    <row r="132" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F132" s="3" t="s">
         <v>478</v>
       </c>
@@ -7683,7 +7690,7 @@
       <c r="O132" s="6"/>
       <c r="S132" s="12"/>
     </row>
-    <row r="133" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F133" s="3" t="s">
         <v>479</v>
       </c>
@@ -7696,7 +7703,7 @@
       <c r="O133" s="6"/>
       <c r="S133" s="12"/>
     </row>
-    <row r="134" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F134" s="3" t="s">
         <v>480</v>
       </c>
@@ -7709,7 +7716,7 @@
       <c r="O134" s="6"/>
       <c r="S134" s="12"/>
     </row>
-    <row r="135" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F135" s="3" t="s">
         <v>481</v>
       </c>
@@ -7722,7 +7729,7 @@
       <c r="O135" s="6"/>
       <c r="S135" s="12"/>
     </row>
-    <row r="136" spans="6:19" s="3" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="6:19" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="F136" s="3" t="s">
         <v>482</v>
       </c>
@@ -7735,7 +7742,7 @@
       <c r="O136" s="6"/>
       <c r="S136" s="12"/>
     </row>
-    <row r="137" spans="6:19" s="3" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="6:19" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="F137" s="3" t="s">
         <v>483</v>
       </c>
@@ -7748,7 +7755,7 @@
       <c r="O137" s="6"/>
       <c r="S137" s="12"/>
     </row>
-    <row r="138" spans="6:19" s="3" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="6:19" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="F138" s="3" t="s">
         <v>484</v>
       </c>
@@ -7774,7 +7781,7 @@
       <c r="O139" s="6"/>
       <c r="S139" s="12"/>
     </row>
-    <row r="140" spans="6:19" s="3" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="6:19" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="F140" s="3" t="s">
         <v>486</v>
       </c>
@@ -7787,7 +7794,7 @@
       <c r="O140" s="6"/>
       <c r="S140" s="12"/>
     </row>
-    <row r="141" spans="6:19" s="3" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="6:19" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="F141" s="3" t="s">
         <v>487</v>
       </c>
@@ -7800,7 +7807,7 @@
       <c r="O141" s="6"/>
       <c r="S141" s="12"/>
     </row>
-    <row r="142" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F142" s="3" t="s">
         <v>488</v>
       </c>
@@ -7813,7 +7820,7 @@
       <c r="O142" s="6"/>
       <c r="S142" s="12"/>
     </row>
-    <row r="143" spans="6:19" s="3" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="6:19" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="F143" s="3" t="s">
         <v>489</v>
       </c>
@@ -7826,7 +7833,7 @@
       <c r="O143" s="6"/>
       <c r="S143" s="12"/>
     </row>
-    <row r="144" spans="6:19" s="3" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="6:19" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="F144" s="3" t="s">
         <v>490</v>
       </c>
@@ -7839,7 +7846,7 @@
       <c r="O144" s="6"/>
       <c r="S144" s="12"/>
     </row>
-    <row r="145" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F145" s="3" t="s">
         <v>491</v>
       </c>
@@ -7852,7 +7859,7 @@
       <c r="O145" s="6"/>
       <c r="S145" s="12"/>
     </row>
-    <row r="146" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F146" s="3" t="s">
         <v>492</v>
       </c>
@@ -7865,7 +7872,7 @@
       <c r="O146" s="6"/>
       <c r="S146" s="12"/>
     </row>
-    <row r="147" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F147" s="3" t="s">
         <v>493</v>
       </c>
@@ -7878,7 +7885,7 @@
       <c r="O147" s="6"/>
       <c r="S147" s="12"/>
     </row>
-    <row r="148" spans="6:19" s="3" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="6:19" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="F148" s="3" t="s">
         <v>494</v>
       </c>
@@ -7891,7 +7898,7 @@
       <c r="O148" s="6"/>
       <c r="S148" s="12"/>
     </row>
-    <row r="149" spans="6:19" s="3" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="6:19" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="F149" s="3" t="s">
         <v>495</v>
       </c>
@@ -7904,7 +7911,7 @@
       <c r="O149" s="6"/>
       <c r="S149" s="12"/>
     </row>
-    <row r="150" spans="6:19" s="3" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="6:19" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="F150" s="3" t="s">
         <v>496</v>
       </c>
@@ -7917,7 +7924,7 @@
       <c r="O150" s="6"/>
       <c r="S150" s="12"/>
     </row>
-    <row r="151" spans="6:19" s="3" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="6:19" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="F151" s="3" t="s">
         <v>497</v>
       </c>
@@ -7930,7 +7937,7 @@
       <c r="O151" s="6"/>
       <c r="S151" s="12"/>
     </row>
-    <row r="152" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F152" s="3" t="s">
         <v>498</v>
       </c>
@@ -7943,7 +7950,7 @@
       <c r="O152" s="6"/>
       <c r="S152" s="12"/>
     </row>
-    <row r="153" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F153" s="3" t="s">
         <v>499</v>
       </c>
@@ -7956,7 +7963,7 @@
       <c r="O153" s="6"/>
       <c r="S153" s="12"/>
     </row>
-    <row r="154" spans="6:19" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="6:19" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="F154" s="3" t="s">
         <v>500</v>
       </c>
@@ -7969,7 +7976,7 @@
       <c r="O154" s="6"/>
       <c r="S154" s="12"/>
     </row>
-    <row r="155" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F155" s="3" t="s">
         <v>501</v>
       </c>
@@ -7982,7 +7989,7 @@
       <c r="O155" s="6"/>
       <c r="S155" s="12"/>
     </row>
-    <row r="156" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F156" s="3" t="s">
         <v>502</v>
       </c>
@@ -7995,7 +8002,7 @@
       <c r="O156" s="6"/>
       <c r="S156" s="12"/>
     </row>
-    <row r="157" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F157" s="3" t="s">
         <v>503</v>
       </c>
@@ -8008,7 +8015,7 @@
       <c r="O157" s="6"/>
       <c r="S157" s="12"/>
     </row>
-    <row r="158" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F158" s="3" t="s">
         <v>504</v>
       </c>
@@ -8021,7 +8028,7 @@
       <c r="O158" s="6"/>
       <c r="S158" s="12"/>
     </row>
-    <row r="159" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F159" s="3" t="s">
         <v>505</v>
       </c>
@@ -8034,7 +8041,7 @@
       <c r="O159" s="6"/>
       <c r="S159" s="12"/>
     </row>
-    <row r="160" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F160" s="3" t="s">
         <v>506</v>
       </c>
@@ -8047,7 +8054,7 @@
       <c r="O160" s="6"/>
       <c r="S160" s="12"/>
     </row>
-    <row r="161" spans="6:19" s="3" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="6:19" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="F161" s="3" t="s">
         <v>507</v>
       </c>
@@ -8060,7 +8067,7 @@
       <c r="O161" s="6"/>
       <c r="S161" s="12"/>
     </row>
-    <row r="162" spans="6:19" s="3" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="6:19" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="F162" s="3" t="s">
         <v>508</v>
       </c>
@@ -8073,7 +8080,7 @@
       <c r="O162" s="6"/>
       <c r="S162" s="12"/>
     </row>
-    <row r="163" spans="6:19" s="3" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="6:19" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="F163" s="3" t="s">
         <v>509</v>
       </c>
@@ -8086,7 +8093,7 @@
       <c r="O163" s="6"/>
       <c r="S163" s="12"/>
     </row>
-    <row r="164" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F164" s="3" t="s">
         <v>625</v>
       </c>
@@ -8099,7 +8106,7 @@
       <c r="O164" s="10"/>
       <c r="S164" s="12"/>
     </row>
-    <row r="165" spans="6:19" s="3" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="6:19" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="F165" s="3" t="s">
         <v>510</v>
       </c>
@@ -8112,7 +8119,7 @@
       <c r="O165" s="6"/>
       <c r="S165" s="12"/>
     </row>
-    <row r="166" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F166" s="3" t="s">
         <v>511</v>
       </c>
@@ -8125,7 +8132,7 @@
       <c r="O166" s="6"/>
       <c r="S166" s="12"/>
     </row>
-    <row r="167" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F167" s="3" t="s">
         <v>512</v>
       </c>
@@ -8138,7 +8145,7 @@
       <c r="O167" s="6"/>
       <c r="S167" s="12"/>
     </row>
-    <row r="168" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F168" s="3" t="s">
         <v>513</v>
       </c>
@@ -8151,7 +8158,7 @@
       <c r="O168" s="6"/>
       <c r="S168" s="12"/>
     </row>
-    <row r="169" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F169" s="3" t="s">
         <v>514</v>
       </c>
@@ -8164,7 +8171,7 @@
       <c r="O169" s="6"/>
       <c r="S169" s="12"/>
     </row>
-    <row r="170" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F170" s="3" t="s">
         <v>515</v>
       </c>
@@ -8177,7 +8184,7 @@
       <c r="O170" s="6"/>
       <c r="S170" s="12"/>
     </row>
-    <row r="171" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F171" s="3" t="s">
         <v>516</v>
       </c>
@@ -8190,7 +8197,7 @@
       <c r="O171" s="6"/>
       <c r="S171" s="12"/>
     </row>
-    <row r="172" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F172" s="3" t="s">
         <v>517</v>
       </c>
@@ -8203,7 +8210,7 @@
       <c r="O172" s="6"/>
       <c r="S172" s="12"/>
     </row>
-    <row r="173" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F173" s="3" t="s">
         <v>518</v>
       </c>
@@ -8216,7 +8223,7 @@
       <c r="O173" s="6"/>
       <c r="S173" s="12"/>
     </row>
-    <row r="174" spans="6:19" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="6:19" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="F174" s="3" t="s">
         <v>519</v>
       </c>
@@ -8229,7 +8236,7 @@
       <c r="O174" s="6"/>
       <c r="S174" s="12"/>
     </row>
-    <row r="175" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F175" s="3" t="s">
         <v>520</v>
       </c>
@@ -8242,7 +8249,7 @@
       <c r="O175" s="6"/>
       <c r="S175" s="12"/>
     </row>
-    <row r="176" spans="6:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="6:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F176" s="3" t="s">
         <v>521</v>
       </c>
@@ -8255,7 +8262,7 @@
       <c r="O176" s="6"/>
       <c r="S176" s="12"/>
     </row>
-    <row r="177" spans="1:19" s="3" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="F177" s="3" t="s">
         <v>522</v>
       </c>
@@ -8268,7 +8275,7 @@
       <c r="O177" s="6"/>
       <c r="S177" s="12"/>
     </row>
-    <row r="178" spans="1:19" s="3" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="F178" s="3" t="s">
         <v>523</v>
       </c>
@@ -8281,7 +8288,7 @@
       <c r="O178" s="6"/>
       <c r="S178" s="12"/>
     </row>
-    <row r="179" spans="1:19" s="3" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="F179" s="3" t="s">
         <v>524</v>
       </c>
@@ -8294,7 +8301,7 @@
       <c r="O179" s="6"/>
       <c r="S179" s="12"/>
     </row>
-    <row r="180" spans="1:19" s="3" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="F180" s="3" t="s">
         <v>525</v>
       </c>
@@ -8307,7 +8314,7 @@
       <c r="O180" s="10"/>
       <c r="S180" s="12"/>
     </row>
-    <row r="181" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>102</v>
       </c>

</xml_diff>